<commit_message>
Operation Chaining 5ns vivado report aggiornati
</commit_message>
<xml_diff>
--- a/reports/vivado/OperationChaining5nsSolution/power/OperationChaining5nsDSPPowerReport.xlsx
+++ b/reports/vivado/OperationChaining5nsSolution/power/OperationChaining5nsDSPPowerReport.xlsx
@@ -172,7 +172,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
-        <v>2.787977282423526E-4</v>
+        <v>2.9166883905418217E-4</v>
       </c>
       <c r="B2" t="s" s="4">
         <v>8</v>
@@ -198,7 +198,7 @@
     </row>
     <row r="3" outlineLevel="1">
       <c r="A3" t="n" s="5">
-        <v>1.3646436855196953E-4</v>
+        <v>1.398509048158303E-4</v>
       </c>
       <c r="B3" t="s" s="4">
         <v>10</v>
@@ -219,12 +219,12 @@
         <v>13</v>
       </c>
       <c r="H3" t="n" s="2">
-        <v>6.162764072418213</v>
+        <v>6.290065765380859</v>
       </c>
     </row>
     <row r="4" outlineLevel="1">
       <c r="A4" t="n" s="5">
-        <v>1.1004078260157257E-4</v>
+        <v>1.1952534259762615E-4</v>
       </c>
       <c r="B4" t="s" s="4">
         <v>14</v>
@@ -245,7 +245,7 @@
         <v>13</v>
       </c>
       <c r="H4" t="n" s="2">
-        <v>4.95597505569458</v>
+        <v>5.308176040649414</v>
       </c>
     </row>
     <row r="5" outlineLevel="1">

</xml_diff>